<commit_message>
update code all time complexity comments and analysis
</commit_message>
<xml_diff>
--- a/performance_results.xlsx
+++ b/performance_results.xlsx
@@ -79,399 +79,399 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="B2" s="0">
-        <v>2E-06</v>
+        <v>3E-06</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="B3" s="0">
-        <v>2.3E-05</v>
+        <v>2.9E-05</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>3001</v>
+        <v>3000</v>
       </c>
       <c r="B4" s="0">
-        <v>8E-06</v>
+        <v>1.3E-05</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>4001</v>
+        <v>4000</v>
       </c>
       <c r="B5" s="0">
-        <v>8.999999999999999E-06</v>
+        <v>1.4999999999999999E-05</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>5001</v>
+        <v>5000</v>
       </c>
       <c r="B6" s="0">
-        <v>1.2E-05</v>
+        <v>1.7999999999999997E-05</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>6001</v>
+        <v>6000</v>
       </c>
       <c r="B7" s="0">
-        <v>1.4E-05</v>
+        <v>2E-05</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>7001</v>
+        <v>7000</v>
       </c>
       <c r="B8" s="0">
-        <v>1.9E-05</v>
+        <v>2.2E-05</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>8001</v>
+        <v>8000</v>
       </c>
       <c r="B9" s="0">
-        <v>1.9E-05</v>
+        <v>2.5E-05</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>9001</v>
+        <v>9000</v>
       </c>
       <c r="B10" s="0">
-        <v>2.4E-05</v>
+        <v>2.6E-05</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>10001</v>
+        <v>10000</v>
       </c>
       <c r="B11" s="0">
-        <v>2.3E-05</v>
+        <v>2.6E-05</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>11001</v>
+        <v>11000</v>
       </c>
       <c r="B12" s="0">
-        <v>2.4E-05</v>
+        <v>3.1E-05</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>12001</v>
+        <v>12000</v>
       </c>
       <c r="B13" s="0">
-        <v>2.6E-05</v>
+        <v>3.5000000000000004E-05</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>13001</v>
+        <v>13000</v>
       </c>
       <c r="B14" s="0">
-        <v>2.8E-05</v>
+        <v>3.9E-05</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>14001</v>
+        <v>14000</v>
       </c>
       <c r="B15" s="0">
-        <v>3.1E-05</v>
+        <v>4.4E-05</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>15001</v>
+        <v>15000</v>
       </c>
       <c r="B16" s="0">
-        <v>3.3E-05</v>
+        <v>5.5E-05</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>16001</v>
+        <v>16000</v>
       </c>
       <c r="B17" s="0">
-        <v>3.5999999999999994E-05</v>
+        <v>5.1E-05</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>17001</v>
+        <v>17000</v>
       </c>
       <c r="B18" s="0">
-        <v>3.8E-05</v>
+        <v>5.5E-05</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>18001</v>
+        <v>18000</v>
       </c>
       <c r="B19" s="0">
-        <v>4.1E-05</v>
+        <v>5E-05</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>19001</v>
+        <v>19000</v>
       </c>
       <c r="B20" s="0">
-        <v>4.2999999999999995E-05</v>
+        <v>5.9999999999999995E-05</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>20001</v>
+        <v>20000</v>
       </c>
       <c r="B21" s="0">
-        <v>4.4E-05</v>
+        <v>6.500000000000001E-05</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>21001</v>
+        <v>21000</v>
       </c>
       <c r="B22" s="0">
-        <v>5.9999999999999995E-05</v>
+        <v>5.9E-05</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>22001</v>
+        <v>22000</v>
       </c>
       <c r="B23" s="0">
-        <v>9.1E-05</v>
+        <v>8.599999999999999E-05</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>23001</v>
+        <v>23000</v>
       </c>
       <c r="B24" s="0">
-        <v>9.2E-05</v>
+        <v>9.3E-05</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>24001</v>
+        <v>24000</v>
       </c>
       <c r="B25" s="0">
-        <v>9.5E-05</v>
+        <v>9.6E-05</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>25001</v>
+        <v>25000</v>
       </c>
       <c r="B26" s="0">
-        <v>7.8E-05</v>
+        <v>0.000131</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>26001</v>
+        <v>26000</v>
       </c>
       <c r="B27" s="0">
-        <v>8.2E-05</v>
+        <v>0.00010899999999999999</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>27001</v>
+        <v>27000</v>
       </c>
       <c r="B28" s="0">
-        <v>8.7E-05</v>
+        <v>0.000102</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>28001</v>
+        <v>28000</v>
       </c>
       <c r="B29" s="0">
-        <v>8.5E-05</v>
+        <v>9.900000000000001E-05</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>29001</v>
+        <v>29000</v>
       </c>
       <c r="B30" s="0">
-        <v>8.599999999999999E-05</v>
+        <v>0.000114</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>30001</v>
+        <v>30000</v>
       </c>
       <c r="B31" s="0">
-        <v>9.5E-05</v>
+        <v>9.7E-05</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>31001</v>
+        <v>31000</v>
       </c>
       <c r="B32" s="0">
-        <v>0.000101</v>
+        <v>9.5E-05</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>32001</v>
+        <v>32000</v>
       </c>
       <c r="B33" s="0">
-        <v>0.000102</v>
+        <v>0.00011999999999999999</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>33001</v>
+        <v>33000</v>
       </c>
       <c r="B34" s="0">
-        <v>0.0001</v>
+        <v>0.000116</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>34001</v>
+        <v>34000</v>
       </c>
       <c r="B35" s="0">
-        <v>9.800000000000001E-05</v>
+        <v>0.000107</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>35001</v>
+        <v>35000</v>
       </c>
       <c r="B36" s="0">
-        <v>0.000107</v>
+        <v>0.000106</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>36001</v>
+        <v>36000</v>
       </c>
       <c r="B37" s="0">
-        <v>0.000111</v>
+        <v>0.000114</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>37001</v>
+        <v>37000</v>
       </c>
       <c r="B38" s="0">
-        <v>0.000104</v>
+        <v>0.000112</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>38001</v>
+        <v>38000</v>
       </c>
       <c r="B39" s="0">
-        <v>0.000107</v>
+        <v>0.000111</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>39001</v>
+        <v>39000</v>
       </c>
       <c r="B40" s="0">
-        <v>9.900000000000001E-05</v>
+        <v>0.000125</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>40001</v>
+        <v>40000</v>
       </c>
       <c r="B41" s="0">
-        <v>0.000104</v>
+        <v>0.000116</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>41001</v>
+        <v>41000</v>
       </c>
       <c r="B42" s="0">
-        <v>0.00010899999999999999</v>
+        <v>0.000115</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>42001</v>
+        <v>42000</v>
       </c>
       <c r="B43" s="0">
-        <v>0.000123</v>
+        <v>0.000122</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>43001</v>
+        <v>43000</v>
       </c>
       <c r="B44" s="0">
-        <v>0.00011999999999999999</v>
+        <v>0.000122</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>44001</v>
+        <v>44000</v>
       </c>
       <c r="B45" s="0">
-        <v>0.000115</v>
+        <v>0.000114</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>45001</v>
+        <v>45000</v>
       </c>
       <c r="B46" s="0">
-        <v>0.00011300000000000001</v>
+        <v>0.000124</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>46001</v>
+        <v>46000</v>
       </c>
       <c r="B47" s="0">
-        <v>0.000116</v>
+        <v>0.000125</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>47001</v>
+        <v>47000</v>
       </c>
       <c r="B48" s="0">
-        <v>0.000116</v>
+        <v>0.00013800000000000002</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>48001</v>
+        <v>48000</v>
       </c>
       <c r="B49" s="0">
-        <v>0.000122</v>
+        <v>0.00013800000000000002</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>49001</v>
+        <v>49000</v>
       </c>
       <c r="B50" s="0">
-        <v>0.000125</v>
+        <v>0.000135</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>50001</v>
+        <v>50000</v>
       </c>
       <c r="B51" s="0">
         <v>0.00014299999999999998</v>
@@ -479,82 +479,82 @@
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>51001</v>
+        <v>51000</v>
       </c>
       <c r="B52" s="0">
-        <v>0.00014000000000000001</v>
+        <v>0.00013800000000000002</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0">
-        <v>52001</v>
+        <v>52000</v>
       </c>
       <c r="B53" s="0">
-        <v>0.00014099999999999998</v>
+        <v>0.000136</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>53001</v>
+        <v>53000</v>
       </c>
       <c r="B54" s="0">
-        <v>0.00013700000000000002</v>
+        <v>0.000158</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>54001</v>
+        <v>54000</v>
       </c>
       <c r="B55" s="0">
-        <v>0.00014000000000000001</v>
+        <v>0.00016700000000000002</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>55001</v>
+        <v>55000</v>
       </c>
       <c r="B56" s="0">
-        <v>0.00014000000000000001</v>
+        <v>0.00016</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>56001</v>
+        <v>56000</v>
       </c>
       <c r="B57" s="0">
-        <v>0.00014199999999999998</v>
+        <v>0.000163</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>57001</v>
+        <v>57000</v>
       </c>
       <c r="B58" s="0">
-        <v>0.00016</v>
+        <v>0.000156</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0">
-        <v>58001</v>
+        <v>58000</v>
       </c>
       <c r="B59" s="0">
-        <v>0.000163</v>
+        <v>0.00016700000000000002</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0">
-        <v>59001</v>
+        <v>59000</v>
       </c>
       <c r="B60" s="0">
-        <v>0.00015900000000000002</v>
+        <v>0.000154</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0">
-        <v>60001</v>
+        <v>60000</v>
       </c>
       <c r="B61" s="0">
-        <v>0.000152</v>
+        <v>0.000156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>